<commit_message>
Updates to lookup exercise readme
</commit_message>
<xml_diff>
--- a/Excel/projects/budget_lookups/metro_budget_exercise.xlsx
+++ b/Excel/projects/budget_lookups/metro_budget_exercise.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary van Valkenburg\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{99C8BFA1-FB13-4840-8D2B-9D0C7B0608DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{19ED61FC-0AAB-4DAC-83F6-00D6AC42053B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="135" yWindow="90" windowWidth="21877" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -264,7 +264,7 @@
     <t>FY19</t>
   </si>
   <si>
-    <t>Question 7</t>
+    <t>Question 8</t>
   </si>
   <si>
     <t>Rank:</t>
@@ -273,7 +273,7 @@
     <t>Pct</t>
   </si>
   <si>
-    <t>Question 8</t>
+    <t>Question 9</t>
   </si>
   <si>
     <t>Metro Nashville government department name</t>
@@ -1178,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1256,9 +1256,6 @@
       <c r="C2">
         <v>341243679.13</v>
       </c>
-      <c r="D2">
-        <v>-15396420.869999999</v>
-      </c>
       <c r="E2" s="5"/>
       <c r="G2">
         <v>382685200</v>
@@ -1266,9 +1263,6 @@
       <c r="H2">
         <v>346340810.81999999</v>
       </c>
-      <c r="I2">
-        <v>-36344389.179999702</v>
-      </c>
       <c r="J2" s="5"/>
       <c r="L2">
         <v>376548600</v>
@@ -1276,9 +1270,6 @@
       <c r="M2">
         <v>355279492.22999901</v>
       </c>
-      <c r="N2">
-        <v>-21269107.77</v>
-      </c>
       <c r="O2" s="5"/>
     </row>
     <row r="3" spans="1:16">
@@ -1291,9 +1282,6 @@
       <c r="C3">
         <v>321214.59000000003</v>
       </c>
-      <c r="D3">
-        <v>-7585.4099999999698</v>
-      </c>
       <c r="E3" s="5"/>
       <c r="G3">
         <v>334800</v>
@@ -1301,9 +1289,6 @@
       <c r="H3">
         <v>312433.70999999897</v>
       </c>
-      <c r="I3">
-        <v>-22366.29</v>
-      </c>
       <c r="J3" s="5"/>
       <c r="L3">
         <v>322700</v>
@@ -1311,9 +1296,6 @@
       <c r="M3">
         <v>322263.03999999998</v>
       </c>
-      <c r="N3">
-        <v>-436.96000000001999</v>
-      </c>
       <c r="O3" s="5"/>
     </row>
     <row r="4" spans="1:16">
@@ -1326,9 +1308,6 @@
       <c r="C4">
         <v>3115157.5599999898</v>
       </c>
-      <c r="D4">
-        <v>-15442.440000000401</v>
-      </c>
       <c r="E4" s="5"/>
       <c r="G4">
         <v>3652300</v>
@@ -1336,9 +1315,6 @@
       <c r="H4">
         <v>3589693.2099999902</v>
       </c>
-      <c r="I4">
-        <v>-62606.790000000903</v>
-      </c>
       <c r="J4" s="5"/>
       <c r="L4">
         <v>3662400</v>
@@ -1346,9 +1322,6 @@
       <c r="M4">
         <v>3564983.04999999</v>
       </c>
-      <c r="N4">
-        <v>-97416.950000001103</v>
-      </c>
       <c r="O4" s="5"/>
     </row>
     <row r="5" spans="1:16">
@@ -1361,9 +1334,6 @@
       <c r="C5">
         <v>6947552.6699999999</v>
       </c>
-      <c r="D5">
-        <v>-723147.33</v>
-      </c>
       <c r="E5" s="5"/>
       <c r="G5">
         <v>7968300</v>
@@ -1371,9 +1341,6 @@
       <c r="H5">
         <v>7020609.3200000003</v>
       </c>
-      <c r="I5">
-        <v>-947690.67999999702</v>
-      </c>
       <c r="J5" s="5"/>
       <c r="L5">
         <v>7759600</v>
@@ -1381,9 +1348,6 @@
       <c r="M5">
         <v>7497322.9100000001</v>
       </c>
-      <c r="N5">
-        <v>-262277.08999999898</v>
-      </c>
       <c r="O5" s="5"/>
     </row>
     <row r="6" spans="1:16">
@@ -1396,9 +1360,6 @@
       <c r="C6">
         <v>385908.52</v>
       </c>
-      <c r="D6">
-        <v>-23391.479999999901</v>
-      </c>
       <c r="E6" s="5"/>
       <c r="G6">
         <v>428500</v>
@@ -1406,9 +1367,6 @@
       <c r="H6">
         <v>427758.64</v>
       </c>
-      <c r="I6">
-        <v>-741.35999999998603</v>
-      </c>
       <c r="J6" s="5"/>
       <c r="L6">
         <v>445200</v>
@@ -1416,9 +1374,6 @@
       <c r="M6">
         <v>445114.28999999899</v>
       </c>
-      <c r="N6">
-        <v>-85.710000000079106</v>
-      </c>
       <c r="O6" s="5"/>
     </row>
     <row r="7" spans="1:16">
@@ -1431,9 +1386,6 @@
       <c r="C7">
         <v>2946071.21</v>
       </c>
-      <c r="D7">
-        <v>-382928.79</v>
-      </c>
       <c r="E7" s="5"/>
       <c r="G7">
         <v>3390900</v>
@@ -1441,9 +1393,6 @@
       <c r="H7">
         <v>3051483.41</v>
       </c>
-      <c r="I7">
-        <v>-339416.58999999898</v>
-      </c>
       <c r="J7" s="5"/>
       <c r="L7">
         <v>3345200</v>
@@ -1451,9 +1400,6 @@
       <c r="M7">
         <v>2946440.08</v>
       </c>
-      <c r="N7">
-        <v>-398759.91999999899</v>
-      </c>
       <c r="O7" s="5"/>
     </row>
     <row r="8" spans="1:16">
@@ -1466,9 +1412,6 @@
       <c r="C8">
         <v>1315623.30999999</v>
       </c>
-      <c r="D8">
-        <v>-236476.69</v>
-      </c>
       <c r="E8" s="5"/>
       <c r="G8">
         <v>1590700</v>
@@ -1476,9 +1419,6 @@
       <c r="H8">
         <v>1383905.98999999</v>
       </c>
-      <c r="I8">
-        <v>-206794.01</v>
-      </c>
       <c r="J8" s="5"/>
       <c r="L8">
         <v>1579300</v>
@@ -1486,9 +1426,6 @@
       <c r="M8">
         <v>1337735.3199999901</v>
       </c>
-      <c r="N8">
-        <v>-241564.68</v>
-      </c>
       <c r="O8" s="5"/>
     </row>
     <row r="9" spans="1:16">
@@ -1501,9 +1438,6 @@
       <c r="C9">
         <v>8952825.2799999993</v>
       </c>
-      <c r="D9">
-        <v>-396574.71999999997</v>
-      </c>
       <c r="E9" s="5"/>
       <c r="G9">
         <v>11073700</v>
@@ -1511,9 +1445,6 @@
       <c r="H9">
         <v>9929059.5199999996</v>
       </c>
-      <c r="I9">
-        <v>-1144640.48</v>
-      </c>
       <c r="J9" s="5"/>
       <c r="L9">
         <v>10790500</v>
@@ -1521,9 +1452,6 @@
       <c r="M9">
         <v>9993599.52999999</v>
       </c>
-      <c r="N9">
-        <v>-796900.47000000405</v>
-      </c>
       <c r="O9" s="5"/>
     </row>
     <row r="10" spans="1:16">
@@ -1536,9 +1464,6 @@
       <c r="C10">
         <v>407090.37</v>
       </c>
-      <c r="D10">
-        <v>-36209.629999999903</v>
-      </c>
       <c r="E10" s="5"/>
       <c r="G10">
         <v>495200</v>
@@ -1546,9 +1471,6 @@
       <c r="H10">
         <v>467907.84000000003</v>
       </c>
-      <c r="I10">
-        <v>-27292.159999999902</v>
-      </c>
       <c r="J10" s="5"/>
       <c r="L10">
         <v>487500</v>
@@ -1556,9 +1478,6 @@
       <c r="M10">
         <v>478318.92</v>
       </c>
-      <c r="N10">
-        <v>-9181.0800000000108</v>
-      </c>
       <c r="O10" s="5"/>
     </row>
     <row r="11" spans="1:16">
@@ -1571,9 +1490,6 @@
       <c r="C11">
         <v>0</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
       <c r="E11" s="5"/>
       <c r="G11">
         <v>0</v>
@@ -1581,9 +1497,6 @@
       <c r="H11">
         <v>0</v>
       </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
       <c r="J11" s="5"/>
       <c r="L11">
         <v>375000</v>
@@ -1591,9 +1504,6 @@
       <c r="M11">
         <v>63771.91</v>
       </c>
-      <c r="N11">
-        <v>-311228.08999999898</v>
-      </c>
       <c r="O11" s="5"/>
     </row>
     <row r="12" spans="1:16">
@@ -1606,9 +1516,6 @@
       <c r="C12">
         <v>4066595.33</v>
       </c>
-      <c r="D12">
-        <v>-214304.669999998</v>
-      </c>
       <c r="E12" s="5"/>
       <c r="G12">
         <v>4700400</v>
@@ -1616,9 +1523,6 @@
       <c r="H12">
         <v>4205555.5999999996</v>
       </c>
-      <c r="I12">
-        <v>-494844.39999999799</v>
-      </c>
       <c r="J12" s="5"/>
       <c r="L12">
         <v>4677800</v>
@@ -1626,9 +1530,6 @@
       <c r="M12">
         <v>4371713.1399999997</v>
       </c>
-      <c r="N12">
-        <v>-306086.86</v>
-      </c>
       <c r="O12" s="5"/>
     </row>
     <row r="13" spans="1:16">
@@ -1641,9 +1542,6 @@
       <c r="C13">
         <v>5772288.3300000001</v>
       </c>
-      <c r="D13">
-        <v>-75511.669999999896</v>
-      </c>
       <c r="E13" s="5"/>
       <c r="G13">
         <v>6223700</v>
@@ -1651,9 +1549,6 @@
       <c r="H13">
         <v>5909077.9399999902</v>
       </c>
-      <c r="I13">
-        <v>-314622.06</v>
-      </c>
       <c r="J13" s="5"/>
       <c r="L13">
         <v>6207300</v>
@@ -1661,9 +1556,6 @@
       <c r="M13">
         <v>6056976.6699999999</v>
       </c>
-      <c r="N13">
-        <v>-150323.329999999</v>
-      </c>
       <c r="O13" s="5"/>
     </row>
     <row r="14" spans="1:16">
@@ -1676,9 +1568,6 @@
       <c r="C14">
         <v>505017.37</v>
       </c>
-      <c r="D14">
-        <v>-6982.6299999998801</v>
-      </c>
       <c r="E14" s="5"/>
       <c r="G14">
         <v>530500</v>
@@ -1686,9 +1575,6 @@
       <c r="H14">
         <v>524402.98</v>
       </c>
-      <c r="I14">
-        <v>-6097.0199999999004</v>
-      </c>
       <c r="J14" s="5"/>
       <c r="L14">
         <v>526200</v>
@@ -1696,9 +1582,6 @@
       <c r="M14">
         <v>504989.88</v>
       </c>
-      <c r="N14">
-        <v>-21210.119999999901</v>
-      </c>
       <c r="O14" s="5"/>
     </row>
     <row r="15" spans="1:16">
@@ -1711,9 +1594,6 @@
       <c r="C15">
         <v>156545919.90000001</v>
       </c>
-      <c r="D15">
-        <v>496819.90000000497</v>
-      </c>
       <c r="E15" s="5"/>
       <c r="G15">
         <v>184167800</v>
@@ -1721,9 +1601,6 @@
       <c r="H15">
         <v>175966389.24999899</v>
       </c>
-      <c r="I15">
-        <v>-8201410.7500000298</v>
-      </c>
       <c r="J15" s="5"/>
       <c r="L15">
         <v>188953500</v>
@@ -1731,9 +1608,6 @@
       <c r="M15">
         <v>184450910.84999901</v>
       </c>
-      <c r="N15">
-        <v>-4502589.1500000302</v>
-      </c>
       <c r="O15" s="5"/>
     </row>
     <row r="16" spans="1:16">
@@ -1746,9 +1620,6 @@
       <c r="C16">
         <v>6522480.4599999897</v>
       </c>
-      <c r="D16">
-        <v>-78219.540000000896</v>
-      </c>
       <c r="E16" s="5"/>
       <c r="G16">
         <v>7352500</v>
@@ -1756,9 +1627,6 @@
       <c r="H16">
         <v>7350464.0800000001</v>
       </c>
-      <c r="I16">
-        <v>-2035.91999999992</v>
-      </c>
       <c r="J16" s="5"/>
       <c r="L16">
         <v>7397200</v>
@@ -1766,9 +1634,6 @@
       <c r="M16">
         <v>7397093</v>
       </c>
-      <c r="N16">
-        <v>-106.999999999068</v>
-      </c>
       <c r="O16" s="5"/>
     </row>
     <row r="17" spans="1:15">
@@ -1781,9 +1646,6 @@
       <c r="C17">
         <v>14439480.050000001</v>
       </c>
-      <c r="D17">
-        <v>-421319.94999999902</v>
-      </c>
       <c r="E17" s="5"/>
       <c r="G17">
         <v>15309700</v>
@@ -1791,9 +1653,6 @@
       <c r="H17">
         <v>14645233.51</v>
       </c>
-      <c r="I17">
-        <v>-664466.49</v>
-      </c>
       <c r="J17" s="5"/>
       <c r="L17">
         <v>15311800</v>
@@ -1801,9 +1660,6 @@
       <c r="M17">
         <v>14346057.039999999</v>
       </c>
-      <c r="N17">
-        <v>-965742.96</v>
-      </c>
       <c r="O17" s="5"/>
     </row>
     <row r="18" spans="1:15">
@@ -1816,9 +1672,6 @@
       <c r="C18">
         <v>2615303.8999999901</v>
       </c>
-      <c r="D18">
-        <v>-149396.1</v>
-      </c>
       <c r="E18" s="5"/>
       <c r="G18">
         <v>2861000</v>
@@ -1826,9 +1679,6 @@
       <c r="H18">
         <v>2671745.94</v>
       </c>
-      <c r="I18">
-        <v>-189254.05999999901</v>
-      </c>
       <c r="J18" s="5"/>
       <c r="L18">
         <v>2910600</v>
@@ -1836,9 +1686,6 @@
       <c r="M18">
         <v>2535637.09</v>
       </c>
-      <c r="N18">
-        <v>-374962.91</v>
-      </c>
       <c r="O18" s="5"/>
     </row>
     <row r="19" spans="1:15">
@@ -1851,9 +1698,6 @@
       <c r="C19">
         <v>8460963.1999999899</v>
       </c>
-      <c r="D19">
-        <v>-376336.800000004</v>
-      </c>
       <c r="E19" s="5"/>
       <c r="G19">
         <v>9713300</v>
@@ -1861,9 +1705,6 @@
       <c r="H19">
         <v>8991707.2399999909</v>
       </c>
-      <c r="I19">
-        <v>-721592.76000000304</v>
-      </c>
       <c r="J19" s="5"/>
       <c r="L19">
         <v>9343000</v>
@@ -1871,9 +1712,6 @@
       <c r="M19">
         <v>8766655.9100000001</v>
       </c>
-      <c r="N19">
-        <v>-576344.08999999403</v>
-      </c>
       <c r="O19" s="5"/>
     </row>
     <row r="20" spans="1:15">
@@ -1886,9 +1724,6 @@
       <c r="C20">
         <v>124384360.159999</v>
       </c>
-      <c r="D20">
-        <v>-1539.8400000184699</v>
-      </c>
       <c r="E20" s="5"/>
       <c r="G20">
         <v>131849400</v>
@@ -1896,9 +1731,6 @@
       <c r="H20">
         <v>131839624.37</v>
       </c>
-      <c r="I20">
-        <v>-9775.6299999654293</v>
-      </c>
       <c r="J20" s="5"/>
       <c r="L20">
         <v>130621400</v>
@@ -1906,9 +1738,6 @@
       <c r="M20">
         <v>130621283.53999899</v>
       </c>
-      <c r="N20">
-        <v>-116.46000003814601</v>
-      </c>
       <c r="O20" s="5"/>
     </row>
     <row r="21" spans="1:15">
@@ -1921,9 +1750,6 @@
       <c r="C21">
         <v>22408587.5499999</v>
       </c>
-      <c r="D21">
-        <v>-1923512.45000002</v>
-      </c>
       <c r="E21" s="5"/>
       <c r="G21">
         <v>24497400</v>
@@ -1931,9 +1757,6 @@
       <c r="H21">
         <v>22655993.629999999</v>
       </c>
-      <c r="I21">
-        <v>-1841406.37</v>
-      </c>
       <c r="J21" s="5"/>
       <c r="L21">
         <v>24323000</v>
@@ -1941,9 +1764,6 @@
       <c r="M21">
         <v>23434073.089999899</v>
       </c>
-      <c r="N21">
-        <v>-888926.91000000294</v>
-      </c>
       <c r="O21" s="5"/>
     </row>
     <row r="22" spans="1:15">
@@ -1956,9 +1776,6 @@
       <c r="C22">
         <v>11412339.8799999</v>
       </c>
-      <c r="D22">
-        <v>-153660.120000002</v>
-      </c>
       <c r="E22" s="5"/>
       <c r="G22">
         <v>11980700</v>
@@ -1966,9 +1783,6 @@
       <c r="H22">
         <v>11791977.9699999</v>
       </c>
-      <c r="I22">
-        <v>-188722.03000000099</v>
-      </c>
       <c r="J22" s="5"/>
       <c r="L22">
         <v>11935200</v>
@@ -1976,9 +1790,6 @@
       <c r="M22">
         <v>11934454.77</v>
       </c>
-      <c r="N22">
-        <v>-745.22999999672095</v>
-      </c>
       <c r="O22" s="5"/>
     </row>
     <row r="23" spans="1:15">
@@ -1991,9 +1802,6 @@
       <c r="C23">
         <v>20036743.4099999</v>
       </c>
-      <c r="D23">
-        <v>-825956.59000001801</v>
-      </c>
       <c r="E23" s="5"/>
       <c r="G23">
         <v>22683800</v>
@@ -2001,9 +1809,6 @@
       <c r="H23">
         <v>21722126.219999898</v>
       </c>
-      <c r="I23">
-        <v>-961673.78000002704</v>
-      </c>
       <c r="J23" s="5"/>
       <c r="L23">
         <v>23220300</v>
@@ -2011,9 +1816,6 @@
       <c r="M23">
         <v>22619057.440000001</v>
       </c>
-      <c r="N23">
-        <v>-601242.55999998702</v>
-      </c>
       <c r="O23" s="5"/>
     </row>
     <row r="24" spans="1:15">
@@ -2026,9 +1828,6 @@
       <c r="C24">
         <v>904969.19</v>
       </c>
-      <c r="D24">
-        <v>-12230.809999999799</v>
-      </c>
       <c r="E24" s="5"/>
       <c r="G24">
         <v>1112700</v>
@@ -2036,9 +1835,6 @@
       <c r="H24">
         <v>1067214.42</v>
       </c>
-      <c r="I24">
-        <v>-45485.579999999798</v>
-      </c>
       <c r="J24" s="5"/>
       <c r="L24">
         <v>1112600</v>
@@ -2046,9 +1842,6 @@
       <c r="M24">
         <v>1112527.1200000001</v>
       </c>
-      <c r="N24">
-        <v>-72.879999999888199</v>
-      </c>
       <c r="O24" s="5"/>
     </row>
     <row r="25" spans="1:15">
@@ -2061,9 +1854,6 @@
       <c r="C25">
         <v>479149.53</v>
       </c>
-      <c r="D25">
-        <v>-4950.4699999999102</v>
-      </c>
       <c r="E25" s="5"/>
       <c r="G25">
         <v>505200</v>
@@ -2071,9 +1861,6 @@
       <c r="H25">
         <v>497194.20999999897</v>
       </c>
-      <c r="I25">
-        <v>-8005.79000000003</v>
-      </c>
       <c r="J25" s="5"/>
       <c r="L25">
         <v>496500</v>
@@ -2081,9 +1868,6 @@
       <c r="M25">
         <v>494775.1</v>
       </c>
-      <c r="N25">
-        <v>-1724.8999999999601</v>
-      </c>
       <c r="O25" s="5"/>
     </row>
     <row r="26" spans="1:15">
@@ -2096,9 +1880,6 @@
       <c r="C26">
         <v>4801960.08</v>
       </c>
-      <c r="D26">
-        <v>-447839.91999999899</v>
-      </c>
       <c r="E26" s="5"/>
       <c r="G26">
         <v>5442200</v>
@@ -2106,9 +1887,6 @@
       <c r="H26">
         <v>5122329.02999999</v>
       </c>
-      <c r="I26">
-        <v>-319870.96999999997</v>
-      </c>
       <c r="J26" s="5"/>
       <c r="L26">
         <v>5430700</v>
@@ -2116,9 +1894,6 @@
       <c r="M26">
         <v>5117235.21</v>
       </c>
-      <c r="N26">
-        <v>-313464.78999999998</v>
-      </c>
       <c r="O26" s="5"/>
     </row>
     <row r="27" spans="1:15">
@@ -2131,9 +1906,6 @@
       <c r="C27">
         <v>0</v>
       </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
       <c r="E27" s="5"/>
       <c r="G27">
         <v>0</v>
@@ -2141,9 +1913,6 @@
       <c r="H27">
         <v>0</v>
       </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
       <c r="J27" s="5"/>
       <c r="L27">
         <v>0</v>
@@ -2151,9 +1920,6 @@
       <c r="M27">
         <v>0</v>
       </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
       <c r="O27" s="5"/>
     </row>
     <row r="28" spans="1:15">
@@ -2166,9 +1932,6 @@
       <c r="C28">
         <v>1250442.02</v>
       </c>
-      <c r="D28">
-        <v>-132457.97999999899</v>
-      </c>
       <c r="E28" s="5"/>
       <c r="G28">
         <v>1545700</v>
@@ -2176,9 +1939,6 @@
       <c r="H28">
         <v>1281335.23</v>
       </c>
-      <c r="I28">
-        <v>-264364.77</v>
-      </c>
       <c r="J28" s="5"/>
       <c r="L28">
         <v>1525900</v>
@@ -2186,9 +1946,6 @@
       <c r="M28">
         <v>1393285.06</v>
       </c>
-      <c r="N28">
-        <v>-132614.93999999901</v>
-      </c>
       <c r="O28" s="5"/>
     </row>
     <row r="29" spans="1:15">
@@ -2201,9 +1958,6 @@
       <c r="C29">
         <v>2523884.71</v>
       </c>
-      <c r="D29">
-        <v>-37915.289999999099</v>
-      </c>
       <c r="E29" s="5"/>
       <c r="G29">
         <v>2779500</v>
@@ -2211,9 +1965,6 @@
       <c r="H29">
         <v>2665264.4399999902</v>
       </c>
-      <c r="I29">
-        <v>-114235.56</v>
-      </c>
       <c r="J29" s="5"/>
       <c r="L29">
         <v>2889900</v>
@@ -2221,9 +1972,6 @@
       <c r="M29">
         <v>2889864.67</v>
       </c>
-      <c r="N29">
-        <v>-35.329999999143098</v>
-      </c>
       <c r="O29" s="5"/>
     </row>
     <row r="30" spans="1:15">
@@ -2236,9 +1984,6 @@
       <c r="C30">
         <v>12030494.1</v>
       </c>
-      <c r="D30">
-        <v>-101705.89999998899</v>
-      </c>
       <c r="E30" s="5"/>
       <c r="G30">
         <v>12735900</v>
@@ -2246,9 +1991,6 @@
       <c r="H30">
         <v>12685514.279999901</v>
       </c>
-      <c r="I30">
-        <v>-50385.720000002497</v>
-      </c>
       <c r="J30" s="5"/>
       <c r="L30">
         <v>12861300</v>
@@ -2256,9 +1998,6 @@
       <c r="M30">
         <v>12826009.609999999</v>
       </c>
-      <c r="N30">
-        <v>-35290.389999991203</v>
-      </c>
       <c r="O30" s="5"/>
     </row>
     <row r="31" spans="1:15">
@@ -2271,9 +2010,6 @@
       <c r="C31">
         <v>1740827.69</v>
       </c>
-      <c r="D31">
-        <v>-24772.309999999299</v>
-      </c>
       <c r="E31" s="5"/>
       <c r="G31">
         <v>1823300</v>
@@ -2281,9 +2017,6 @@
       <c r="H31">
         <v>1762676.85</v>
       </c>
-      <c r="I31">
-        <v>-60623.1499999999</v>
-      </c>
       <c r="J31" s="5"/>
       <c r="L31">
         <v>1870700</v>
@@ -2291,9 +2024,6 @@
       <c r="M31">
         <v>1801391.34</v>
       </c>
-      <c r="N31">
-        <v>-69308.659999999596</v>
-      </c>
       <c r="O31" s="5"/>
     </row>
     <row r="32" spans="1:15">
@@ -2306,9 +2036,6 @@
       <c r="C32">
         <v>5925637.7199999904</v>
       </c>
-      <c r="D32">
-        <v>-73762.280000002094</v>
-      </c>
       <c r="E32" s="5"/>
       <c r="G32">
         <v>6195500</v>
@@ -2316,9 +2043,6 @@
       <c r="H32">
         <v>6084985.4699999997</v>
       </c>
-      <c r="I32">
-        <v>-110514.52999999801</v>
-      </c>
       <c r="J32" s="5"/>
       <c r="L32">
         <v>6157400</v>
@@ -2326,9 +2050,6 @@
       <c r="M32">
         <v>5987572.0199999996</v>
       </c>
-      <c r="N32">
-        <v>-169827.98</v>
-      </c>
       <c r="O32" s="5"/>
     </row>
     <row r="33" spans="1:15">
@@ -2341,9 +2062,6 @@
       <c r="C33">
         <v>920284264.73000002</v>
       </c>
-      <c r="D33">
-        <v>-7418835.2699993802</v>
-      </c>
       <c r="E33" s="5"/>
       <c r="G33">
         <v>979671000</v>
@@ -2351,9 +2069,6 @@
       <c r="H33">
         <v>977068513.48000002</v>
       </c>
-      <c r="I33">
-        <v>-2602486.5200004498</v>
-      </c>
       <c r="J33" s="5"/>
       <c r="L33">
         <v>989572899.99999905</v>
@@ -2361,9 +2076,6 @@
       <c r="M33">
         <v>984116289.40999901</v>
       </c>
-      <c r="N33">
-        <v>-5456610.5900001498</v>
-      </c>
       <c r="O33" s="5"/>
     </row>
     <row r="34" spans="1:15">
@@ -2376,9 +2088,6 @@
       <c r="C34">
         <v>4109958.22</v>
       </c>
-      <c r="D34">
-        <v>-79341.779999998806</v>
-      </c>
       <c r="E34" s="5"/>
       <c r="G34">
         <v>4350600</v>
@@ -2386,9 +2095,6 @@
       <c r="H34">
         <v>4137588.7699999898</v>
       </c>
-      <c r="I34">
-        <v>-213011.23</v>
-      </c>
       <c r="J34" s="5"/>
       <c r="L34">
         <v>4345600</v>
@@ -2396,9 +2102,6 @@
       <c r="M34">
         <v>4229801.51</v>
       </c>
-      <c r="N34">
-        <v>-115798.49</v>
-      </c>
       <c r="O34" s="5"/>
     </row>
     <row r="35" spans="1:15">
@@ -2411,9 +2114,6 @@
       <c r="C35">
         <v>0</v>
       </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
       <c r="E35" s="5"/>
       <c r="G35">
         <v>0</v>
@@ -2421,9 +2121,6 @@
       <c r="H35">
         <v>0</v>
       </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
       <c r="J35" s="5"/>
       <c r="L35">
         <v>0</v>
@@ -2431,9 +2128,6 @@
       <c r="M35">
         <v>0</v>
       </c>
-      <c r="N35">
-        <v>0</v>
-      </c>
       <c r="O35" s="5"/>
     </row>
     <row r="36" spans="1:15">
@@ -2446,9 +2140,6 @@
       <c r="C36">
         <v>735423.27999999898</v>
       </c>
-      <c r="D36">
-        <v>-62776.720000000198</v>
-      </c>
       <c r="E36" s="5"/>
       <c r="G36">
         <v>898700</v>
@@ -2456,9 +2147,6 @@
       <c r="H36">
         <v>740966.94999999902</v>
       </c>
-      <c r="I36">
-        <v>-157733.04999999999</v>
-      </c>
       <c r="J36" s="5"/>
       <c r="L36">
         <v>878300</v>
@@ -2466,9 +2154,6 @@
       <c r="M36">
         <v>777215.28999999899</v>
       </c>
-      <c r="N36">
-        <v>-101084.71</v>
-      </c>
       <c r="O36" s="5"/>
     </row>
     <row r="37" spans="1:15">
@@ -2481,9 +2166,6 @@
       <c r="C37">
         <v>2005447.73999999</v>
       </c>
-      <c r="D37">
-        <v>-82352.260000000693</v>
-      </c>
       <c r="E37" s="5"/>
       <c r="G37">
         <v>2229200</v>
@@ -2491,9 +2173,6 @@
       <c r="H37">
         <v>2118943.21</v>
       </c>
-      <c r="I37">
-        <v>-110256.789999999</v>
-      </c>
       <c r="J37" s="5"/>
       <c r="L37">
         <v>2296900</v>
@@ -2501,9 +2180,6 @@
       <c r="M37">
         <v>2108718.34</v>
       </c>
-      <c r="N37">
-        <v>-188181.66</v>
-      </c>
       <c r="O37" s="5"/>
     </row>
     <row r="38" spans="1:15">
@@ -2516,9 +2192,6 @@
       <c r="C38">
         <v>838669.82</v>
       </c>
-      <c r="D38">
-        <v>-16630.1799999998</v>
-      </c>
       <c r="E38" s="5"/>
       <c r="G38">
         <v>792800</v>
@@ -2526,9 +2199,6 @@
       <c r="H38">
         <v>753451.96</v>
       </c>
-      <c r="I38">
-        <v>-39348.039999999797</v>
-      </c>
       <c r="J38" s="5"/>
       <c r="L38">
         <v>777800</v>
@@ -2536,9 +2206,6 @@
       <c r="M38">
         <v>777663.26</v>
       </c>
-      <c r="N38">
-        <v>-136.73999999987399</v>
-      </c>
       <c r="O38" s="5"/>
     </row>
     <row r="39" spans="1:15">
@@ -2551,9 +2218,6 @@
       <c r="C39">
         <v>813108.87</v>
       </c>
-      <c r="D39">
-        <v>-70791.13</v>
-      </c>
       <c r="E39" s="5"/>
       <c r="G39">
         <v>1294400</v>
@@ -2561,9 +2225,6 @@
       <c r="H39">
         <v>1114242.27999999</v>
       </c>
-      <c r="I39">
-        <v>-180157.72</v>
-      </c>
       <c r="J39" s="5"/>
       <c r="L39">
         <v>1759500</v>
@@ -2571,9 +2232,6 @@
       <c r="M39">
         <v>1680463.8699999901</v>
       </c>
-      <c r="N39">
-        <v>-79036.130000000296</v>
-      </c>
       <c r="O39" s="5"/>
     </row>
     <row r="40" spans="1:15">
@@ -2586,9 +2244,6 @@
       <c r="C40">
         <v>37565141.859999903</v>
       </c>
-      <c r="D40">
-        <v>-816758.14000004495</v>
-      </c>
       <c r="E40" s="5"/>
       <c r="G40">
         <v>39964900</v>
@@ -2596,9 +2251,6 @@
       <c r="H40">
         <v>38095240.189999901</v>
       </c>
-      <c r="I40">
-        <v>-1869659.81</v>
-      </c>
       <c r="J40" s="5"/>
       <c r="L40">
         <v>40216700</v>
@@ -2606,9 +2258,6 @@
       <c r="M40">
         <v>39606263.709999897</v>
       </c>
-      <c r="N40">
-        <v>-610436.29000002099</v>
-      </c>
       <c r="O40" s="5"/>
     </row>
     <row r="41" spans="1:15">
@@ -2621,9 +2270,6 @@
       <c r="C41">
         <v>4409060.2099999897</v>
       </c>
-      <c r="D41">
-        <v>-184239.79</v>
-      </c>
       <c r="E41" s="5"/>
       <c r="G41">
         <v>5089500</v>
@@ -2631,9 +2277,6 @@
       <c r="H41">
         <v>4956043.6699999897</v>
       </c>
-      <c r="I41">
-        <v>-133456.33000000101</v>
-      </c>
       <c r="J41" s="5"/>
       <c r="L41">
         <v>4799900</v>
@@ -2641,9 +2284,6 @@
       <c r="M41">
         <v>4717822.6500000004</v>
       </c>
-      <c r="N41">
-        <v>-82077.349999997707</v>
-      </c>
       <c r="O41" s="5"/>
     </row>
     <row r="42" spans="1:15">
@@ -2656,9 +2296,6 @@
       <c r="C42">
         <v>188551675.67999899</v>
       </c>
-      <c r="D42">
-        <v>-41624.320000201398</v>
-      </c>
       <c r="E42" s="5"/>
       <c r="G42">
         <v>199130300</v>
@@ -2666,9 +2303,6 @@
       <c r="H42">
         <v>196755033.31</v>
       </c>
-      <c r="I42">
-        <v>-2375266.6899999301</v>
-      </c>
       <c r="J42" s="5"/>
       <c r="L42">
         <v>199954600</v>
@@ -2676,9 +2310,6 @@
       <c r="M42">
         <v>199954563.74999899</v>
       </c>
-      <c r="N42">
-        <v>-36.250000059604602</v>
-      </c>
       <c r="O42" s="5"/>
     </row>
     <row r="43" spans="1:15">
@@ -2691,9 +2322,6 @@
       <c r="C43">
         <v>7968645.8300000001</v>
       </c>
-      <c r="D43">
-        <v>-166754.16999999899</v>
-      </c>
       <c r="E43" s="5"/>
       <c r="G43">
         <v>8560800</v>
@@ -2701,9 +2329,6 @@
       <c r="H43">
         <v>8171472.0199999996</v>
       </c>
-      <c r="I43">
-        <v>-389327.979999998</v>
-      </c>
       <c r="J43" s="5"/>
       <c r="L43">
         <v>8497500</v>
@@ -2711,9 +2336,6 @@
       <c r="M43">
         <v>8150982.5699999901</v>
       </c>
-      <c r="N43">
-        <v>-346517.43</v>
-      </c>
       <c r="O43" s="5"/>
     </row>
     <row r="44" spans="1:15">
@@ -2726,9 +2348,6 @@
       <c r="C44">
         <v>29789104.379999999</v>
       </c>
-      <c r="D44">
-        <v>-294095.61999999301</v>
-      </c>
       <c r="E44" s="5"/>
       <c r="G44">
         <v>31040700</v>
@@ -2736,9 +2355,6 @@
       <c r="H44">
         <v>30793711.48</v>
       </c>
-      <c r="I44">
-        <v>-246988.51999998</v>
-      </c>
       <c r="J44" s="5"/>
       <c r="L44">
         <v>31282200</v>
@@ -2746,9 +2362,6 @@
       <c r="M44">
         <v>31282141.25</v>
       </c>
-      <c r="N44">
-        <v>-58.749999988824101</v>
-      </c>
       <c r="O44" s="5"/>
     </row>
     <row r="45" spans="1:15">
@@ -2761,9 +2374,6 @@
       <c r="C45">
         <v>54589584.0499999</v>
       </c>
-      <c r="D45">
-        <v>-712015.95000000997</v>
-      </c>
       <c r="E45" s="5"/>
       <c r="G45">
         <v>56792200</v>
@@ -2771,9 +2381,6 @@
       <c r="H45">
         <v>54594953.959999897</v>
       </c>
-      <c r="I45">
-        <v>-2197246.0400000098</v>
-      </c>
       <c r="J45" s="5"/>
       <c r="L45">
         <v>56027100</v>
@@ -2781,9 +2388,6 @@
       <c r="M45">
         <v>55386549.6599999</v>
       </c>
-      <c r="N45">
-        <v>-640550.34000001801</v>
-      </c>
       <c r="O45" s="5"/>
     </row>
     <row r="46" spans="1:15">
@@ -2796,9 +2400,6 @@
       <c r="C46">
         <v>258322.43</v>
       </c>
-      <c r="D46">
-        <v>-777.57000000000698</v>
-      </c>
       <c r="E46" s="5"/>
       <c r="G46">
         <v>266000</v>
@@ -2806,9 +2407,6 @@
       <c r="H46">
         <v>257402.90999999901</v>
       </c>
-      <c r="I46">
-        <v>-8597.0900000000202</v>
-      </c>
       <c r="J46" s="5"/>
       <c r="L46">
         <v>267100</v>
@@ -2816,9 +2414,6 @@
       <c r="M46">
         <v>254753.15999999901</v>
       </c>
-      <c r="N46">
-        <v>-12346.84</v>
-      </c>
       <c r="O46" s="5"/>
     </row>
     <row r="47" spans="1:15">
@@ -2831,9 +2426,6 @@
       <c r="C47">
         <v>70378426.719999999</v>
       </c>
-      <c r="D47">
-        <v>-12273.279999956399</v>
-      </c>
       <c r="E47" s="5"/>
       <c r="G47">
         <v>73467000</v>
@@ -2841,9 +2433,6 @@
       <c r="H47">
         <v>73442541.659999996</v>
       </c>
-      <c r="I47">
-        <v>-24458.339999988599</v>
-      </c>
       <c r="J47" s="5"/>
       <c r="L47">
         <v>75072800</v>
@@ -2851,9 +2440,6 @@
       <c r="M47">
         <v>75050829.179999903</v>
       </c>
-      <c r="N47">
-        <v>-21970.8200000822</v>
-      </c>
       <c r="O47" s="5"/>
     </row>
     <row r="48" spans="1:15">
@@ -2866,9 +2452,6 @@
       <c r="C48">
         <v>6527352.5699999901</v>
       </c>
-      <c r="D48">
-        <v>-209747.43</v>
-      </c>
       <c r="E48" s="5"/>
       <c r="G48">
         <v>7214700</v>
@@ -2876,9 +2459,6 @@
       <c r="H48">
         <v>6922072.5599999996</v>
       </c>
-      <c r="I48">
-        <v>-292627.43999999802</v>
-      </c>
       <c r="J48" s="5"/>
       <c r="L48">
         <v>7289800</v>
@@ -2886,9 +2466,6 @@
       <c r="M48">
         <v>6882350.23999999</v>
       </c>
-      <c r="N48">
-        <v>-407449.76000000199</v>
-      </c>
       <c r="O48" s="5"/>
     </row>
     <row r="49" spans="1:15">
@@ -2901,9 +2478,6 @@
       <c r="C49">
         <v>90499.43</v>
       </c>
-      <c r="D49">
-        <v>-1700.5699999999899</v>
-      </c>
       <c r="E49" s="5"/>
       <c r="G49">
         <v>102600</v>
@@ -2911,9 +2485,6 @@
       <c r="H49">
         <v>95466.880000000005</v>
       </c>
-      <c r="I49">
-        <v>-7133.1199999999799</v>
-      </c>
       <c r="J49" s="5"/>
       <c r="L49">
         <v>0</v>
@@ -2921,9 +2492,6 @@
       <c r="M49">
         <v>0</v>
       </c>
-      <c r="N49">
-        <v>0</v>
-      </c>
       <c r="O49" s="5"/>
     </row>
     <row r="50" spans="1:15">
@@ -2936,9 +2504,6 @@
       <c r="C50">
         <v>832600</v>
       </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
       <c r="E50" s="5"/>
       <c r="G50">
         <v>859100</v>
@@ -2946,9 +2511,6 @@
       <c r="H50">
         <v>859100</v>
       </c>
-      <c r="I50">
-        <v>0</v>
-      </c>
       <c r="J50" s="5"/>
       <c r="L50">
         <v>843200</v>
@@ -2956,9 +2518,6 @@
       <c r="M50">
         <v>843200</v>
       </c>
-      <c r="N50">
-        <v>0</v>
-      </c>
       <c r="O50" s="5"/>
     </row>
     <row r="51" spans="1:15">
@@ -2971,9 +2530,6 @@
       <c r="C51">
         <v>8499425.3399999905</v>
       </c>
-      <c r="D51">
-        <v>-110074.660000002</v>
-      </c>
       <c r="E51" s="5"/>
       <c r="G51">
         <v>8925500</v>
@@ -2981,9 +2537,6 @@
       <c r="H51">
         <v>8599059.6199999992</v>
       </c>
-      <c r="I51">
-        <v>-326440.38</v>
-      </c>
       <c r="J51" s="5"/>
       <c r="L51">
         <v>8833900</v>
@@ -2991,9 +2544,6 @@
       <c r="M51">
         <v>8735843.3100000005</v>
       </c>
-      <c r="N51">
-        <v>-98056.689999999406</v>
-      </c>
       <c r="O51" s="5"/>
     </row>
     <row r="52" spans="1:15">
@@ -3006,9 +2556,6 @@
       <c r="C52">
         <v>2254684.7999999998</v>
       </c>
-      <c r="D52">
-        <v>-196315.19999999899</v>
-      </c>
       <c r="E52" s="5"/>
       <c r="G52">
         <v>2440700</v>
@@ -3016,18 +2563,12 @@
       <c r="H52">
         <v>2204672.88</v>
       </c>
-      <c r="I52">
-        <v>-236027.11999999901</v>
-      </c>
       <c r="J52" s="5"/>
       <c r="L52">
         <v>2321600</v>
       </c>
       <c r="M52">
         <v>2056835.26</v>
-      </c>
-      <c r="N52">
-        <v>-264764.74</v>
       </c>
       <c r="O52" s="5"/>
     </row>
@@ -3191,10 +2732,10 @@
       </c>
     </row>
     <row r="83" spans="1:7">
-      <c r="B83" t="s">
+      <c r="B83" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="1" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>